<commit_message>
Reindex operation for dataframes
</commit_message>
<xml_diff>
--- a/Data_Sources_and_Preparation/Data and Sources.xlsx
+++ b/Data_Sources_and_Preparation/Data and Sources.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="106">
   <si>
     <t xml:space="preserve">Economic Policy Uncertainty </t>
   </si>
@@ -336,13 +336,22 @@
   <si>
     <t>Subject : Consumer Price Index &gt; All items &gt; Total &gt; Total
 Measure : Index 2010=100,</t>
+  </si>
+  <si>
+    <t>https://www.oecd-ilibrary.org/economics/data/prices/producer-prices_data-00535-en</t>
+  </si>
+  <si>
+    <t>Subject: Economic activities - Total producer prices - Manufacturing ?</t>
+  </si>
+  <si>
+    <t>Turkiye Cin ve Ingiltere'nin aynı bazda oldugu bir PPI yok. Cin'nin tek oldugu bu PPI cesidi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,6 +364,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="162"/>
@@ -461,10 +479,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -492,8 +511,10 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -552,13 +573,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>28576</xdr:colOff>
+      <xdr:colOff>35503</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>448441</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>523876</xdr:colOff>
+      <xdr:colOff>530803</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>161571</xdr:rowOff>
     </xdr:to>
@@ -577,8 +598,46 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17030701" y="4972816"/>
-          <a:ext cx="4762500" cy="2646830"/>
+          <a:off x="17035030" y="4958096"/>
+          <a:ext cx="4762500" cy="2636439"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>339436</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>7117</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>444032</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>94563</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3567545" y="7620190"/>
+          <a:ext cx="6172887" cy="4063700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -853,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="I18" zoomScale="110" zoomScaleNormal="90" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A33" zoomScale="110" zoomScaleNormal="90" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1469,7 +1528,9 @@
       <c r="C23" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="7"/>
+      <c r="D23" s="7" t="s">
+        <v>104</v>
+      </c>
       <c r="E23" s="7" t="s">
         <v>86</v>
       </c>
@@ -1512,6 +1573,9 @@
       <c r="I24" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="J24" s="15" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="25" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
@@ -1669,12 +1733,21 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C34" s="13"/>
     </row>
+    <row r="42" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B42" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C42" s="13"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J24" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>